<commit_message>
add airflow scheduler to automate webscrape and write to excel
</commit_message>
<xml_diff>
--- a/clothing_links.xlsx
+++ b/clothing_links.xlsx
@@ -17,7 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,10 +441,30 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.4</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.3</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>link</t>
         </is>
@@ -453,7 +477,19 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>https://prixworkshop.com/products/98-denim-jacket-gunmetal?variant=44590905000150</t>
         </is>
@@ -466,7 +502,19 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>https://prixworkshop.com/products/knight-dress-black?variant=42417948459222</t>
         </is>
@@ -479,7 +527,19 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>https://prixworkshop.com/products/tarmac-works-mazda-rx7</t>
         </is>
@@ -496,7 +556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,6 +580,11 @@
           <t>item_price_regular</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>updated_time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -537,8 +602,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$160.00 CAD</t>
-        </is>
+          <t>$155.00 CAD</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>45768.43399544809</v>
       </c>
     </row>
     <row r="3">
@@ -557,8 +625,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$131.00 CAD</t>
-        </is>
+          <t>$127.00 CAD</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45768.43402195397</v>
       </c>
     </row>
     <row r="4">
@@ -577,8 +648,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$21.00 CAD</t>
-        </is>
+          <t>$20.00 CAD</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45768.4340465211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>